<commit_message>
sửa import excel sản phẩm
</commit_message>
<xml_diff>
--- a/public/excel_sample/product-sample.xlsx
+++ b/public/excel_sample/product-sample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Tên sản phẩm</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Giá</t>
   </si>
   <si>
-    <t>Mô tả</t>
-  </si>
-  <si>
     <t>Giảm giá</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
   </si>
   <si>
     <t>Test Excel 1</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit.</t>
   </si>
   <si>
     <t>LG</t>
@@ -119,9 +113,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,21 +395,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,79 +425,67 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
       </c>
       <c r="B2">
         <v>10000000</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
       </c>
       <c r="B3">
         <v>15000000</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>12000000</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
+      <c r="C4">
         <v>5</v>
       </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
       <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
         <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>